<commit_message>
#13 change db design
</commit_message>
<xml_diff>
--- a/docs/DB設計書/DB設計書.xlsx
+++ b/docs/DB設計書/DB設計書.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="15075" windowHeight="9870" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="15075" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="サマリ" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="221">
   <si>
     <t>エンティティ定義書　サマリ</t>
   </si>
@@ -52,7 +52,7 @@
     <t>作成日</t>
   </si>
   <si>
-    <t>2017/07/13</t>
+    <t>2017/07/18</t>
   </si>
   <si>
     <t>エンティティ一覧</t>
@@ -285,22 +285,28 @@
     <t>name</t>
   </si>
   <si>
+    <t>担当者名</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>郵便番号</t>
+  </si>
+  <si>
+    <t>postal_code</t>
+  </si>
+  <si>
+    <t>VARCHAR(7)</t>
+  </si>
+  <si>
+    <t>住所1</t>
+  </si>
+  <si>
+    <t>address_1</t>
+  </si>
+  <si>
     <t>VARCHAR(100)</t>
-  </si>
-  <si>
-    <t>郵便番号</t>
-  </si>
-  <si>
-    <t>postal_code</t>
-  </si>
-  <si>
-    <t>VARCHAR(7)</t>
-  </si>
-  <si>
-    <t>住所1</t>
-  </si>
-  <si>
-    <t>address_1</t>
   </si>
   <si>
     <t>住所2</t>
@@ -393,7 +399,8 @@
     <t>spec</t>
   </si>
   <si>
-    <t>display_typ</t>
+    <t>0:表示しない_x000D_
+3:表示する</t>
   </si>
   <si>
     <t>発注先ID</t>
@@ -402,7 +409,7 @@
     <t>send_order_customer_id</t>
   </si>
   <si>
-    <t>material_id,deleted_at,receive_order_customer_id,part_number,color_number_code,color_number_tint,display_typ</t>
+    <t>material_id,deleted_at,receive_order_customer_id,part_number,color_number_code,color_number_tint,display_type</t>
   </si>
   <si>
     <t>商品に紐づく材料ID</t>
@@ -489,7 +496,7 @@
     <t>size</t>
   </si>
   <si>
-    <t>指図数量</t>
+    <t>数量</t>
   </si>
   <si>
     <t>instruction_quantity</t>
@@ -531,6 +538,18 @@
     <t>freight_fee</t>
   </si>
   <si>
+    <t>運送便</t>
+  </si>
+  <si>
+    <t>freight_service</t>
+  </si>
+  <si>
+    <t>送り先</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
     <t>メモ</t>
   </si>
   <si>
@@ -573,10 +592,10 @@
     <t>進捗状況.請求</t>
   </si>
   <si>
-    <t>proguress_claim</t>
-  </si>
-  <si>
-    <t>receive_order_detail_id,deleted_at,receive_order_id,part_number,product_id,size,estimated_shipping_date,progress_arrival,progress_cutting,progress_interruption,progress_sewing,progress_shipment,proguress_claim</t>
+    <t>progress_claim</t>
+  </si>
+  <si>
+    <t>receive_order_detail_id,deleted_at,receive_order_id,part_number,product_id,size,estimated_shipping_date,progress_arrival,progress_cutting,progress_interruption,progress_sewing,progress_shipment,progress_claim</t>
   </si>
   <si>
     <t>in_out_order_detail_id</t>
@@ -624,15 +643,18 @@
     <t>send_order_id</t>
   </si>
   <si>
-    <t>数量</t>
-  </si>
-  <si>
     <t>quantity</t>
   </si>
   <si>
     <t>send_order_detail_id,deleted_at,send_order_id,receive_order_detail_id,part_number,product_id,status,size</t>
   </si>
   <si>
+    <t>0:未発注_x000D_
+1:発注_x000D_
+2:一部入荷_x000D_
+3:入荷済み</t>
+  </si>
+  <si>
     <t>send_order_id,deleted_at,receive_order_id,receive_order_customer_id,status</t>
   </si>
   <si>
@@ -640,9 +662,6 @@
   </si>
   <si>
     <t>stock_id</t>
-  </si>
-  <si>
-    <t>customeri_id</t>
   </si>
   <si>
     <t>入出庫区分</t>
@@ -695,7 +714,7 @@
     <t>受発注明細ID</t>
   </si>
   <si>
-    <t>stock_id,customeri_id,material_id,in_out_type,in_out_date</t>
+    <t>stock_id,customer_id,material_id,in_out_type,in_out_date</t>
   </si>
 </sst>
 </file>
@@ -1387,7 +1406,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1634,6 +1653,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1661,17 +1683,17 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1976,7 +1998,7 @@
   </sheetPr>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -2660,10 +2682,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D14" s="62" t="s">
         <v>48</v>
@@ -2749,7 +2771,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D18" s="58" t="s">
         <v>48</v>
@@ -2767,13 +2789,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D19" s="58" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E19" s="58"/>
       <c r="F19" s="67" t="s">
@@ -2788,10 +2810,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D20" s="58" t="s">
         <v>66</v>
@@ -2800,8 +2822,8 @@
       <c r="F20" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="94" t="s">
-        <v>186</v>
+      <c r="G20" s="93" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12" thickBot="1">
@@ -2809,19 +2831,19 @@
         <v>8</v>
       </c>
       <c r="B21" s="60" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C21" s="60" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D21" s="60" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E21" s="60"/>
       <c r="F21" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="92" t="s">
+      <c r="G21" s="94" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2855,7 +2877,7 @@
       </c>
       <c r="B25" s="56"/>
       <c r="C25" s="74" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D25" s="75"/>
       <c r="E25" s="76"/>
@@ -2878,10 +2900,10 @@
         <v>70</v>
       </c>
       <c r="D28" s="73"/>
-      <c r="E28" s="90" t="s">
+      <c r="E28" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="F28" s="93"/>
+      <c r="F28" s="92"/>
       <c r="G28" s="64" t="s">
         <v>76</v>
       </c>
@@ -2893,14 +2915,14 @@
       <c r="B29" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="82" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="83"/>
-      <c r="E29" s="82" t="s">
+      <c r="C29" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="84"/>
+      <c r="E29" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="83"/>
+      <c r="F29" s="84"/>
       <c r="G29" s="57" t="s">
         <v>81</v>
       </c>
@@ -2921,10 +2943,10 @@
         <v>70</v>
       </c>
       <c r="D32" s="73"/>
-      <c r="E32" s="90" t="s">
+      <c r="E32" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="93"/>
+      <c r="F32" s="92"/>
       <c r="G32" s="64" t="s">
         <v>79</v>
       </c>
@@ -2936,16 +2958,16 @@
       <c r="B33" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="88" t="s">
-        <v>139</v>
-      </c>
-      <c r="D33" s="89"/>
-      <c r="E33" s="88" t="s">
+      <c r="C33" s="89" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" s="90"/>
+      <c r="E33" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="89"/>
+      <c r="F33" s="90"/>
       <c r="G33" s="63" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="12" thickBot="1">
@@ -2955,16 +2977,16 @@
       <c r="B34" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="86" t="s">
-        <v>139</v>
-      </c>
-      <c r="D34" s="87"/>
-      <c r="E34" s="86" t="s">
+      <c r="C34" s="87" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="88"/>
+      <c r="E34" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="87"/>
+      <c r="F34" s="88"/>
       <c r="G34" s="61" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3162,10 +3184,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D14" s="62" t="s">
         <v>48</v>
@@ -3248,10 +3270,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D18" s="58" t="s">
         <v>48</v>
@@ -3269,10 +3291,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D19" s="58" t="s">
         <v>48</v>
@@ -3292,10 +3314,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D20" s="58" t="s">
         <v>66</v>
@@ -3315,10 +3337,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D21" s="58" t="s">
         <v>59</v>
@@ -3336,10 +3358,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D22" s="58" t="s">
         <v>59</v>
@@ -3357,10 +3379,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D23" s="58" t="s">
         <v>48</v>
@@ -3370,7 +3392,7 @@
         <v>39</v>
       </c>
       <c r="G23" s="68" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -3378,10 +3400,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="58" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>59</v>
@@ -3391,7 +3413,7 @@
         <v>39</v>
       </c>
       <c r="G24" s="68" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3399,10 +3421,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>59</v>
@@ -3420,10 +3442,10 @@
         <v>13</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D26" s="58" t="s">
         <v>66</v>
@@ -3443,13 +3465,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="58" t="s">
-        <v>195</v>
+        <v>153</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E27" s="58" t="s">
         <v>60</v>
@@ -3466,13 +3488,13 @@
         <v>15</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="E28" s="58"/>
       <c r="F28" s="67" t="s">
@@ -3487,10 +3509,10 @@
         <v>16</v>
       </c>
       <c r="B29" s="60" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C29" s="60" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D29" s="60" t="s">
         <v>66</v>
@@ -3499,7 +3521,7 @@
       <c r="F29" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="G29" s="92" t="s">
+      <c r="G29" s="94" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3533,7 +3555,7 @@
       </c>
       <c r="B33" s="56"/>
       <c r="C33" s="74" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D33" s="75"/>
       <c r="E33" s="76"/>
@@ -3556,10 +3578,10 @@
         <v>70</v>
       </c>
       <c r="D36" s="73"/>
-      <c r="E36" s="90" t="s">
+      <c r="E36" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="93"/>
+      <c r="F36" s="92"/>
       <c r="G36" s="64" t="s">
         <v>76</v>
       </c>
@@ -3571,16 +3593,16 @@
       <c r="B37" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="88" t="s">
-        <v>137</v>
-      </c>
-      <c r="D37" s="89"/>
-      <c r="E37" s="88" t="s">
+      <c r="C37" s="89" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" s="90"/>
+      <c r="E37" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="F37" s="89"/>
+      <c r="F37" s="90"/>
       <c r="G37" s="63" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="12" thickBot="1">
@@ -3590,16 +3612,16 @@
       <c r="B38" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="86" t="s">
-        <v>194</v>
-      </c>
-      <c r="D38" s="87"/>
-      <c r="E38" s="86" t="s">
+      <c r="C38" s="87" t="s">
+        <v>200</v>
+      </c>
+      <c r="D38" s="88"/>
+      <c r="E38" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="87"/>
+      <c r="F38" s="88"/>
       <c r="G38" s="61" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="12" thickBot="1">
@@ -3618,10 +3640,10 @@
         <v>70</v>
       </c>
       <c r="D41" s="73"/>
-      <c r="E41" s="90" t="s">
+      <c r="E41" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="93"/>
+      <c r="F41" s="92"/>
       <c r="G41" s="64" t="s">
         <v>79</v>
       </c>
@@ -3633,16 +3655,16 @@
       <c r="B42" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="82" t="s">
-        <v>192</v>
-      </c>
-      <c r="D42" s="83"/>
-      <c r="E42" s="82" t="s">
+      <c r="C42" s="83" t="s">
+        <v>198</v>
+      </c>
+      <c r="D42" s="84"/>
+      <c r="E42" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="83"/>
+      <c r="F42" s="84"/>
       <c r="G42" s="57" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3840,10 +3862,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D14" s="62" t="s">
         <v>48</v>
@@ -3926,10 +3948,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D18" s="58" t="s">
         <v>48</v>
@@ -3950,7 +3972,7 @@
         <v>80</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D19" s="58" t="s">
         <v>48</v>
@@ -3963,15 +3985,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12" thickBot="1">
+    <row r="20" spans="1:7" ht="45.75" thickBot="1">
       <c r="A20" s="25">
         <v>7</v>
       </c>
       <c r="B20" s="60" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C20" s="60" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D20" s="60" t="s">
         <v>66</v>
@@ -3980,8 +4002,8 @@
       <c r="F20" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="92" t="s">
-        <v>39</v>
+      <c r="G20" s="70" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="12" thickBot="1">
@@ -4014,7 +4036,7 @@
       </c>
       <c r="B24" s="56"/>
       <c r="C24" s="74" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D24" s="75"/>
       <c r="E24" s="76"/>
@@ -4037,10 +4059,10 @@
         <v>70</v>
       </c>
       <c r="D27" s="73"/>
-      <c r="E27" s="90" t="s">
+      <c r="E27" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="93"/>
+      <c r="F27" s="92"/>
       <c r="G27" s="64" t="s">
         <v>76</v>
       </c>
@@ -4052,14 +4074,14 @@
       <c r="B28" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="88" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="89"/>
-      <c r="E28" s="88" t="s">
+      <c r="C28" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="90"/>
+      <c r="E28" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="89"/>
+      <c r="F28" s="90"/>
       <c r="G28" s="63" t="s">
         <v>81</v>
       </c>
@@ -4071,16 +4093,16 @@
       <c r="B29" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="86" t="s">
-        <v>139</v>
-      </c>
-      <c r="D29" s="87"/>
-      <c r="E29" s="86" t="s">
+      <c r="C29" s="87" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="88"/>
+      <c r="E29" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="87"/>
+      <c r="F29" s="88"/>
       <c r="G29" s="61" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="12" thickBot="1">
@@ -4099,10 +4121,10 @@
         <v>70</v>
       </c>
       <c r="D32" s="73"/>
-      <c r="E32" s="90" t="s">
+      <c r="E32" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="93"/>
+      <c r="F32" s="92"/>
       <c r="G32" s="64" t="s">
         <v>79</v>
       </c>
@@ -4114,16 +4136,16 @@
       <c r="B33" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="82" t="s">
-        <v>194</v>
-      </c>
-      <c r="D33" s="83"/>
-      <c r="E33" s="82" t="s">
+      <c r="C33" s="83" t="s">
+        <v>200</v>
+      </c>
+      <c r="D33" s="84"/>
+      <c r="E33" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="83"/>
+      <c r="F33" s="84"/>
       <c r="G33" s="57" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4321,10 +4343,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="D14" s="62" t="s">
         <v>48</v>
@@ -4410,7 +4432,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>201</v>
+        <v>81</v>
       </c>
       <c r="D18" s="58" t="s">
         <v>48</v>
@@ -4430,10 +4452,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D19" s="58" t="s">
         <v>48</v>
@@ -4453,10 +4475,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D20" s="58" t="s">
         <v>66</v>
@@ -4467,8 +4489,8 @@
       <c r="F20" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="94" t="s">
-        <v>204</v>
+      <c r="G20" s="93" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4476,13 +4498,13 @@
         <v>8</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D21" s="58" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E21" s="58" t="s">
         <v>60</v>
@@ -4499,13 +4521,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E22" s="58"/>
       <c r="F22" s="67" t="s">
@@ -4520,13 +4542,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D23" s="58" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E23" s="58"/>
       <c r="F23" s="67" t="s">
@@ -4541,10 +4563,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="58" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>66</v>
@@ -4553,8 +4575,8 @@
       <c r="F24" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="94" t="s">
-        <v>213</v>
+      <c r="G24" s="93" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -4562,10 +4584,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>48</v>
@@ -4586,16 +4608,16 @@
         <v>4</v>
       </c>
       <c r="C26" s="60" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D26" s="60" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="E26" s="60"/>
       <c r="F26" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="G26" s="92" t="s">
+      <c r="G26" s="94" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4629,7 +4651,7 @@
       </c>
       <c r="B30" s="56"/>
       <c r="C30" s="74" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D30" s="75"/>
       <c r="E30" s="76"/>
@@ -4652,10 +4674,10 @@
         <v>70</v>
       </c>
       <c r="D33" s="73"/>
-      <c r="E33" s="90" t="s">
+      <c r="E33" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="F33" s="91"/>
+      <c r="F33" s="95"/>
       <c r="G33" s="64" t="s">
         <v>76</v>
       </c>
@@ -4667,16 +4689,16 @@
       <c r="B34" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="88" t="s">
-        <v>181</v>
-      </c>
-      <c r="D34" s="89"/>
-      <c r="E34" s="88" t="s">
+      <c r="C34" s="89" t="s">
+        <v>187</v>
+      </c>
+      <c r="D34" s="90"/>
+      <c r="E34" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="89"/>
+      <c r="F34" s="90"/>
       <c r="G34" s="63" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="12" thickBot="1">
@@ -4686,16 +4708,16 @@
       <c r="B35" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="86" t="s">
-        <v>181</v>
-      </c>
-      <c r="D35" s="87"/>
-      <c r="E35" s="86" t="s">
+      <c r="C35" s="87" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" s="88"/>
+      <c r="E35" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="F35" s="87"/>
+      <c r="F35" s="88"/>
       <c r="G35" s="61" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="12" thickBot="1">
@@ -4917,7 +4939,7 @@
       <c r="B12" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="96" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="26"/>
@@ -4996,7 +5018,7 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -5416,7 +5438,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5664,7 +5686,7 @@
         <v>83</v>
       </c>
       <c r="D18" s="58" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E18" s="58" t="s">
         <v>60</v>
@@ -5681,13 +5703,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="58" t="s">
-        <v>86</v>
-      </c>
       <c r="D19" s="58" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="E19" s="58"/>
       <c r="F19" s="67" t="s">
@@ -5702,13 +5724,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="58" t="s">
         <v>88</v>
-      </c>
-      <c r="C20" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="58" t="s">
-        <v>84</v>
       </c>
       <c r="E20" s="58"/>
       <c r="F20" s="67" t="s">
@@ -5723,13 +5745,13 @@
         <v>8</v>
       </c>
       <c r="B21" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="D21" s="58" t="s">
         <v>91</v>
-      </c>
-      <c r="D21" s="58" t="s">
-        <v>84</v>
       </c>
       <c r="E21" s="58"/>
       <c r="F21" s="67" t="s">
@@ -5750,7 +5772,7 @@
         <v>93</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E22" s="58"/>
       <c r="F22" s="67" t="s">
@@ -5765,13 +5787,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="58" t="s">
+      <c r="D23" s="58" t="s">
         <v>96</v>
-      </c>
-      <c r="D23" s="58" t="s">
-        <v>63</v>
       </c>
       <c r="E23" s="58"/>
       <c r="F23" s="67" t="s">
@@ -5802,203 +5824,224 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45.75" thickBot="1">
-      <c r="A25" s="25">
+    <row r="25" spans="1:7">
+      <c r="A25" s="22">
         <v>12</v>
       </c>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="60" t="s">
+      <c r="D25" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="58"/>
+      <c r="F25" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45.75" thickBot="1">
+      <c r="A26" s="25">
+        <v>13</v>
+      </c>
+      <c r="B26" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="60"/>
-      <c r="F25" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="G25" s="70" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="12" thickBot="1">
-      <c r="A27" s="21" t="s">
+      <c r="E26" s="60"/>
+      <c r="F26" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="70" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="12" thickBot="1">
+      <c r="A28" s="21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="31" t="s">
+    <row r="29" spans="1:7">
+      <c r="A29" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="B29" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="71" t="s">
+      <c r="C29" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="72"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="52" t="s">
+      <c r="D29" s="72"/>
+      <c r="E29" s="73"/>
+      <c r="F29" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="64" t="s">
+      <c r="G29" s="64" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A29" s="55">
+    <row r="30" spans="1:7" ht="14.25" thickBot="1">
+      <c r="A30" s="55">
         <v>1</v>
       </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="74" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="75"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="57"/>
-    </row>
-    <row r="31" spans="1:7" ht="12" thickBot="1">
-      <c r="A31" s="21" t="s">
+      <c r="B30" s="56"/>
+      <c r="C30" s="74" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="75"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="57"/>
+    </row>
+    <row r="32" spans="1:7" ht="12" thickBot="1">
+      <c r="A32" s="21" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A32" s="35" t="s">
+    <row r="33" spans="1:7" ht="12" thickBot="1">
+      <c r="A33" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B33" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="77" t="s">
+      <c r="C33" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="78"/>
-      <c r="E32" s="79" t="s">
+      <c r="D33" s="78"/>
+      <c r="E33" s="79" t="s">
         <v>75</v>
       </c>
-      <c r="F32" s="80"/>
-      <c r="G32" s="37" t="s">
+      <c r="F33" s="82"/>
+      <c r="G33" s="37" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="12" thickBot="1">
-      <c r="A34" s="21" t="s">
+    <row r="35" spans="1:7" ht="12" thickBot="1">
+      <c r="A35" s="21" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="31" t="s">
+    <row r="36" spans="1:7" ht="13.5">
+      <c r="A36" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="52" t="s">
+      <c r="B36" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="71" t="s">
+      <c r="C36" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="73"/>
-      <c r="E35" s="90" t="s">
+      <c r="D36" s="73"/>
+      <c r="E36" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="F35" s="91"/>
-      <c r="G35" s="64" t="s">
+      <c r="F36" s="92"/>
+      <c r="G36" s="64" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="28">
+    <row r="37" spans="1:7">
+      <c r="A37" s="28">
         <v>1</v>
       </c>
-      <c r="B36" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="88" t="s">
+      <c r="B37" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="89"/>
-      <c r="E36" s="88" t="s">
+      <c r="D37" s="90"/>
+      <c r="E37" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="89"/>
-      <c r="G36" s="63" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="22">
-        <v>2</v>
-      </c>
-      <c r="B37" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="84" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="85"/>
-      <c r="E37" s="84" t="s">
-        <v>23</v>
-      </c>
-      <c r="F37" s="85"/>
-      <c r="G37" s="59" t="s">
-        <v>103</v>
+      <c r="F37" s="90"/>
+      <c r="G37" s="63" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="22">
+        <v>2</v>
+      </c>
+      <c r="B38" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="86"/>
+      <c r="E38" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="86"/>
+      <c r="G38" s="59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="22">
         <v>3</v>
       </c>
-      <c r="B38" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="84" t="s">
+      <c r="B39" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="D38" s="85"/>
-      <c r="E38" s="84" t="s">
+      <c r="D39" s="86"/>
+      <c r="E39" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="85"/>
-      <c r="G38" s="59" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="12" thickBot="1">
-      <c r="A39" s="25">
+      <c r="F39" s="86"/>
+      <c r="G39" s="59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="12" thickBot="1">
+      <c r="A40" s="25">
         <v>4</v>
       </c>
-      <c r="B39" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="86" t="s">
+      <c r="B40" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="87"/>
-      <c r="E39" s="86" t="s">
+      <c r="D40" s="88"/>
+      <c r="E40" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="F39" s="87"/>
-      <c r="G39" s="61" t="s">
-        <v>103</v>
+      <c r="F40" s="88"/>
+      <c r="G40" s="61" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="E33:F33"/>
     <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -6181,10 +6224,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D14" s="62" t="s">
         <v>48</v>
@@ -6270,7 +6313,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D18" s="58" t="s">
         <v>48</v>
@@ -6288,13 +6331,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D19" s="58" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E19" s="58"/>
       <c r="F19" s="67" t="s">
@@ -6309,10 +6352,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D20" s="58" t="s">
         <v>59</v>
@@ -6332,13 +6375,13 @@
         <v>8</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D21" s="58" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E21" s="58"/>
       <c r="F21" s="67" t="s">
@@ -6353,10 +6396,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D22" s="58" t="s">
         <v>59</v>
@@ -6374,10 +6417,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D23" s="58" t="s">
         <v>66</v>
@@ -6397,13 +6440,13 @@
         <v>11</v>
       </c>
       <c r="B24" s="58" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D24" s="58" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E24" s="58"/>
       <c r="F24" s="67" t="s">
@@ -6413,15 +6456,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="22.5">
       <c r="A25" s="22">
         <v>12</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>66</v>
@@ -6430,8 +6473,8 @@
       <c r="F25" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="68" t="s">
-        <v>39</v>
+      <c r="G25" s="93" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="12" thickBot="1">
@@ -6439,10 +6482,10 @@
         <v>13</v>
       </c>
       <c r="B26" s="60" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C26" s="60" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D26" s="60" t="s">
         <v>48</v>
@@ -6453,7 +6496,7 @@
       <c r="F26" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="G26" s="92" t="s">
+      <c r="G26" s="94" t="s">
         <v>39</v>
       </c>
     </row>
@@ -6487,7 +6530,7 @@
       </c>
       <c r="B30" s="56"/>
       <c r="C30" s="74" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D30" s="75"/>
       <c r="E30" s="76"/>
@@ -6510,10 +6553,10 @@
         <v>70</v>
       </c>
       <c r="D33" s="73"/>
-      <c r="E33" s="90" t="s">
+      <c r="E33" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="F33" s="91"/>
+      <c r="F33" s="95"/>
       <c r="G33" s="64" t="s">
         <v>76</v>
       </c>
@@ -6525,14 +6568,14 @@
       <c r="B34" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="82" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" s="83"/>
-      <c r="E34" s="82" t="s">
+      <c r="C34" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="84"/>
+      <c r="E34" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="83"/>
+      <c r="F34" s="84"/>
       <c r="G34" s="57" t="s">
         <v>81</v>
       </c>
@@ -6553,10 +6596,10 @@
         <v>70</v>
       </c>
       <c r="D37" s="73"/>
-      <c r="E37" s="90" t="s">
+      <c r="E37" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="F37" s="93"/>
+      <c r="F37" s="92"/>
       <c r="G37" s="64" t="s">
         <v>79</v>
       </c>
@@ -6568,16 +6611,16 @@
       <c r="B38" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="82" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" s="83"/>
-      <c r="E38" s="82" t="s">
+      <c r="C38" s="83" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="84"/>
+      <c r="E38" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="F38" s="83"/>
+      <c r="F38" s="84"/>
       <c r="G38" s="57" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -6773,10 +6816,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D14" s="62" t="s">
         <v>48</v>
@@ -6859,10 +6902,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D18" s="58" t="s">
         <v>48</v>
@@ -6880,10 +6923,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D19" s="58" t="s">
         <v>48</v>
@@ -6901,13 +6944,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="60" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C20" s="60" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D20" s="60" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E20" s="60" t="s">
         <v>60</v>
@@ -6915,7 +6958,7 @@
       <c r="F20" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="92" t="s">
+      <c r="G20" s="94" t="s">
         <v>39</v>
       </c>
     </row>
@@ -6949,7 +6992,7 @@
       </c>
       <c r="B24" s="56"/>
       <c r="C24" s="74" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D24" s="75"/>
       <c r="E24" s="76"/>
@@ -6972,10 +7015,10 @@
         <v>70</v>
       </c>
       <c r="D27" s="73"/>
-      <c r="E27" s="90" t="s">
+      <c r="E27" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="93"/>
+      <c r="F27" s="92"/>
       <c r="G27" s="64" t="s">
         <v>76</v>
       </c>
@@ -6987,16 +7030,16 @@
       <c r="B28" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="88" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28" s="89"/>
-      <c r="E28" s="88" t="s">
+      <c r="C28" s="89" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="90"/>
+      <c r="E28" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="89"/>
+      <c r="F28" s="90"/>
       <c r="G28" s="63" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="12" thickBot="1">
@@ -7006,16 +7049,16 @@
       <c r="B29" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="86" t="s">
-        <v>126</v>
-      </c>
-      <c r="D29" s="87"/>
-      <c r="E29" s="86" t="s">
+      <c r="C29" s="87" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="88"/>
+      <c r="E29" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="87"/>
+      <c r="F29" s="88"/>
       <c r="G29" s="61" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="12" thickBot="1">
@@ -7235,10 +7278,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D14" s="62" t="s">
         <v>48</v>
@@ -7324,7 +7367,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D18" s="58" t="s">
         <v>48</v>
@@ -7342,13 +7385,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D19" s="58" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E19" s="58"/>
       <c r="F19" s="67" t="s">
@@ -7363,7 +7406,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C20" s="58" t="s">
         <v>83</v>
@@ -7386,10 +7429,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D21" s="58" t="s">
         <v>59</v>
@@ -7402,15 +7445,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="22.5">
       <c r="A22" s="22">
         <v>9</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D22" s="58" t="s">
         <v>66</v>
@@ -7419,8 +7462,8 @@
       <c r="F22" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="68" t="s">
-        <v>39</v>
+      <c r="G22" s="93" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -7428,10 +7471,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D23" s="58" t="s">
         <v>66</v>
@@ -7451,19 +7494,19 @@
         <v>11</v>
       </c>
       <c r="B24" s="60" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C24" s="60" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D24" s="60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E24" s="60"/>
       <c r="F24" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="92" t="s">
+      <c r="G24" s="94" t="s">
         <v>39</v>
       </c>
     </row>
@@ -7497,7 +7540,7 @@
       </c>
       <c r="B28" s="56"/>
       <c r="C28" s="74" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D28" s="75"/>
       <c r="E28" s="76"/>
@@ -7520,10 +7563,10 @@
         <v>70</v>
       </c>
       <c r="D31" s="73"/>
-      <c r="E31" s="90" t="s">
+      <c r="E31" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="93"/>
+      <c r="F31" s="92"/>
       <c r="G31" s="64" t="s">
         <v>76</v>
       </c>
@@ -7535,14 +7578,14 @@
       <c r="B32" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="82" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" s="83"/>
-      <c r="E32" s="82" t="s">
+      <c r="C32" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="84"/>
+      <c r="E32" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="83"/>
+      <c r="F32" s="84"/>
       <c r="G32" s="57" t="s">
         <v>81</v>
       </c>
@@ -7563,10 +7606,10 @@
         <v>70</v>
       </c>
       <c r="D35" s="73"/>
-      <c r="E35" s="90" t="s">
+      <c r="E35" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="F35" s="91"/>
+      <c r="F35" s="95"/>
       <c r="G35" s="64" t="s">
         <v>79</v>
       </c>
@@ -7578,16 +7621,16 @@
       <c r="B36" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="82" t="s">
-        <v>126</v>
-      </c>
-      <c r="D36" s="83"/>
-      <c r="E36" s="82" t="s">
+      <c r="C36" s="83" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="84"/>
+      <c r="E36" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="83"/>
+      <c r="F36" s="84"/>
       <c r="G36" s="57" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -7627,7 +7670,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7783,10 +7826,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D14" s="62" t="s">
         <v>48</v>
@@ -7869,10 +7912,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D18" s="58" t="s">
         <v>48</v>
@@ -7890,10 +7933,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D19" s="58" t="s">
         <v>66</v>
@@ -7913,10 +7956,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D20" s="58" t="s">
         <v>59</v>
@@ -7934,10 +7977,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D21" s="58" t="s">
         <v>59</v>
@@ -7955,10 +7998,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D22" s="58" t="s">
         <v>48</v>
@@ -7968,7 +8011,7 @@
         <v>39</v>
       </c>
       <c r="G22" s="68" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -7976,10 +8019,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D23" s="58" t="s">
         <v>59</v>
@@ -7989,7 +8032,7 @@
         <v>39</v>
       </c>
       <c r="G23" s="68" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -7997,10 +8040,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="58" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>59</v>
@@ -8018,10 +8061,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>66</v>
@@ -8041,13 +8084,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E26" s="58" t="s">
         <v>60</v>
@@ -8064,13 +8107,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="58" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C27" s="58" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" s="58" t="s">
         <v>155</v>
-      </c>
-      <c r="D27" s="58" t="s">
-        <v>153</v>
       </c>
       <c r="E27" s="58"/>
       <c r="F27" s="67" t="s">
@@ -8085,13 +8128,13 @@
         <v>15</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E28" s="58"/>
       <c r="F28" s="67" t="s">
@@ -8106,13 +8149,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="58" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E29" s="58"/>
       <c r="F29" s="67" t="s">
@@ -8127,13 +8170,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="58" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D30" s="58" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E30" s="58"/>
       <c r="F30" s="67" t="s">
@@ -8148,10 +8191,10 @@
         <v>18</v>
       </c>
       <c r="B31" s="58" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D31" s="58" t="s">
         <v>66</v>
@@ -8171,13 +8214,13 @@
         <v>19</v>
       </c>
       <c r="B32" s="58" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>167</v>
+        <v>59</v>
       </c>
       <c r="E32" s="58"/>
       <c r="F32" s="67" t="s">
@@ -8192,13 +8235,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C33" s="58" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D33" s="58" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E33" s="58"/>
       <c r="F33" s="67" t="s">
@@ -8213,13 +8256,13 @@
         <v>21</v>
       </c>
       <c r="B34" s="58" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C34" s="58" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D34" s="58" t="s">
-        <v>66</v>
+        <v>173</v>
       </c>
       <c r="E34" s="58"/>
       <c r="F34" s="67" t="s">
@@ -8234,10 +8277,10 @@
         <v>22</v>
       </c>
       <c r="B35" s="58" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D35" s="58" t="s">
         <v>66</v>
@@ -8255,10 +8298,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="58" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D36" s="58" t="s">
         <v>66</v>
@@ -8276,10 +8319,10 @@
         <v>24</v>
       </c>
       <c r="B37" s="58" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D37" s="58" t="s">
         <v>66</v>
@@ -8292,182 +8335,224 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12" thickBot="1">
-      <c r="A38" s="25">
+    <row r="38" spans="1:7">
+      <c r="A38" s="22">
         <v>25</v>
       </c>
-      <c r="B38" s="60" t="s">
-        <v>178</v>
-      </c>
-      <c r="C38" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="D38" s="60" t="s">
+      <c r="B38" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="C38" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="D38" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="60"/>
-      <c r="F38" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="G38" s="92" t="s">
+      <c r="E38" s="58"/>
+      <c r="F38" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="22">
+        <v>26</v>
+      </c>
+      <c r="B39" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39" s="58" t="s">
+        <v>183</v>
+      </c>
+      <c r="D39" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="58"/>
+      <c r="F39" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="68" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="12" thickBot="1">
-      <c r="A40" s="21" t="s">
+      <c r="A40" s="25">
+        <v>27</v>
+      </c>
+      <c r="B40" s="60" t="s">
+        <v>184</v>
+      </c>
+      <c r="C40" s="60" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="60"/>
+      <c r="F40" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="G40" s="94" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="12" thickBot="1">
+      <c r="A42" s="21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="31" t="s">
+    <row r="43" spans="1:7">
+      <c r="A43" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="52" t="s">
+      <c r="B43" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="71" t="s">
+      <c r="C43" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="72"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="52" t="s">
+      <c r="D43" s="72"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="G41" s="64" t="s">
+      <c r="G43" s="64" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A42" s="55">
+    <row r="44" spans="1:7" ht="14.25" thickBot="1">
+      <c r="A44" s="55">
         <v>1</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="74" t="s">
-        <v>180</v>
-      </c>
-      <c r="D42" s="75"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="57"/>
-    </row>
-    <row r="44" spans="1:7" ht="12" thickBot="1">
-      <c r="A44" s="21" t="s">
+      <c r="B44" s="56"/>
+      <c r="C44" s="74" t="s">
+        <v>186</v>
+      </c>
+      <c r="D44" s="75"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="57"/>
+    </row>
+    <row r="46" spans="1:7" ht="12" thickBot="1">
+      <c r="A46" s="21" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="13.5">
-      <c r="A45" s="31" t="s">
+    <row r="47" spans="1:7" ht="13.5">
+      <c r="A47" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="52" t="s">
+      <c r="B47" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="71" t="s">
+      <c r="C47" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="73"/>
-      <c r="E45" s="90" t="s">
+      <c r="D47" s="73"/>
+      <c r="E47" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="F45" s="93"/>
-      <c r="G45" s="64" t="s">
+      <c r="F47" s="92"/>
+      <c r="G47" s="64" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12" thickBot="1">
-      <c r="A46" s="55">
+    <row r="48" spans="1:7" ht="12" thickBot="1">
+      <c r="A48" s="55">
         <v>1</v>
       </c>
-      <c r="B46" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="C46" s="82" t="s">
+      <c r="B48" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="83" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="84"/>
+      <c r="E48" s="83" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" s="84"/>
+      <c r="G48" s="57" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="12" thickBot="1">
+      <c r="A50" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="71" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" s="73"/>
+      <c r="E51" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="F51" s="95"/>
+      <c r="G51" s="64" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="28">
+        <v>1</v>
+      </c>
+      <c r="B52" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="89" t="s">
         <v>139</v>
       </c>
-      <c r="D46" s="83"/>
-      <c r="E46" s="82" t="s">
-        <v>27</v>
-      </c>
-      <c r="F46" s="83"/>
-      <c r="G46" s="57" t="s">
+      <c r="D52" s="90"/>
+      <c r="E52" s="89" t="s">
+        <v>33</v>
+      </c>
+      <c r="F52" s="90"/>
+      <c r="G52" s="63" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="12" thickBot="1">
+      <c r="A53" s="25">
+        <v>2</v>
+      </c>
+      <c r="B53" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="87" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="12" thickBot="1">
-      <c r="A48" s="21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="B49" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="C49" s="71" t="s">
-        <v>70</v>
-      </c>
-      <c r="D49" s="73"/>
-      <c r="E49" s="90" t="s">
-        <v>78</v>
-      </c>
-      <c r="F49" s="91"/>
-      <c r="G49" s="64" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="28">
-        <v>1</v>
-      </c>
-      <c r="B50" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="88" t="s">
-        <v>137</v>
-      </c>
-      <c r="D50" s="89"/>
-      <c r="E50" s="88" t="s">
-        <v>33</v>
-      </c>
-      <c r="F50" s="89"/>
-      <c r="G50" s="63" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="12" thickBot="1">
-      <c r="A51" s="25">
-        <v>2</v>
-      </c>
-      <c r="B51" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="C51" s="86" t="s">
-        <v>137</v>
-      </c>
-      <c r="D51" s="87"/>
-      <c r="E51" s="86" t="s">
+      <c r="D53" s="88"/>
+      <c r="E53" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="87"/>
-      <c r="G51" s="61" t="s">
-        <v>137</v>
+      <c r="F53" s="88"/>
+      <c r="G53" s="61" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="C51:D51"/>
     <mergeCell ref="E51:F51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>

</xml_diff>